<commit_message>
8/11 added more changes
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/DataDriven.xlsx
+++ b/src/main/java/com/qa/testdata/DataDriven.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurabh_Dubey\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SeleniumProject\src\main\java\com\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11C9B15-C74A-433E-879A-F3169259E8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C335DB5E-5C17-4A33-9ED9-96F40F0BD35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{22C7AA1A-FC34-4205-AB7B-702C5388C3A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>First Name</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Website Feedback</t>
+  </si>
+  <si>
+    <t>UserName</t>
   </si>
 </sst>
 </file>
@@ -470,87 +473,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A680F680-BC98-413B-BFE8-C67E0B663821}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{27982907-BEBF-4AA4-A8CB-86F160881EFD}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{E63EC1D0-F900-4FAE-9B79-E4BF0CC65BB0}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{6215FD29-3D1C-4C58-950D-01C005F99595}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{27982907-BEBF-4AA4-A8CB-86F160881EFD}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{E63EC1D0-F900-4FAE-9B79-E4BF0CC65BB0}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{6215FD29-3D1C-4C58-950D-01C005F99595}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>